<commit_message>
(Integration Test) House Detail
</commit_message>
<xml_diff>
--- a/Documentation/FHF_TestCases.xlsx
+++ b/Documentation/FHF_TestCases.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Semester9\SEP490\fu-house-finder\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SEP490\fu-house-finder\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C288DFE-6C7B-41DC-B017-4E482FDB6A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="891" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" tabRatio="891" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -28,7 +27,7 @@
     <sheet name="Login" sheetId="15" r:id="rId13"/>
     <sheet name="(Landlord) Upload House Info" sheetId="16" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="198">
   <si>
     <t>Project Name</t>
   </si>
@@ -304,11 +303,393 @@
   <si>
     <t>13/11/2022</t>
   </si>
+  <si>
+    <t>TS_FHF_HouseDetail_001</t>
+  </si>
+  <si>
+    <t>1. Do not login the system
+2. Open report modal
+3. Input data
+4. Click on report button</t>
+  </si>
+  <si>
+    <t>Click report button when not logged in</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_002</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowAlert_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowAlert_002</t>
+  </si>
+  <si>
+    <t>Click report button when  logged in</t>
+  </si>
+  <si>
+    <t>Disable report button when input is empty</t>
+  </si>
+  <si>
+    <t>User see the hidden button and cannot click</t>
+  </si>
+  <si>
+    <t>System disables report button</t>
+  </si>
+  <si>
+    <t>1. Open report modal
+2. Leave the input box empty</t>
+  </si>
+  <si>
+    <t>1. Login the system
+2. Open report modal
+3. Input data
+4. Click on report button</t>
+  </si>
+  <si>
+    <t>User see success alert when click report button</t>
+  </si>
+  <si>
+    <t>System shows the warning alert</t>
+  </si>
+  <si>
+    <t>User see warning alert when click report button</t>
+  </si>
+  <si>
+    <t>System shows the success alert</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_003</t>
+  </si>
+  <si>
+    <t>Verify the show success alert  functionality of House Detail</t>
+  </si>
+  <si>
+    <t>Verify the show warning alert  functionality of House Detail</t>
+  </si>
+  <si>
+    <t>Verify the cancel report  functionality of House Detail</t>
+  </si>
+  <si>
+    <t>Verify the validation  functionality of House Detail</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_CancelReport_001</t>
+  </si>
+  <si>
+    <t>Click cancel button</t>
+  </si>
+  <si>
+    <t>1. Open report modal
+2. Click on cancel button</t>
+  </si>
+  <si>
+    <t>User see report modal close immediately</t>
+  </si>
+  <si>
+    <t>System closes the report modal</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_004</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_005</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowHouseImage_001</t>
+  </si>
+  <si>
+    <t>User see image of house</t>
+  </si>
+  <si>
+    <t>System shows the image of house</t>
+  </si>
+  <si>
+    <t>Load page</t>
+  </si>
+  <si>
+    <t>1. Load page</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_006</t>
+  </si>
+  <si>
+    <t>Verify the show image of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t>Verify the detail landlord of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowLandlord_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User see detail information of landlord </t>
+  </si>
+  <si>
+    <t>System shows the detail information of landlord</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_007</t>
+  </si>
+  <si>
+    <t>Verify the information of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t>System shows the detail information of this house</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User see detail information of this house </t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_008</t>
+  </si>
+  <si>
+    <t>Verify the location of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowLocation_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowInformation_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User see location of house </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System shows the location of house </t>
+  </si>
+  <si>
+    <t>Verify the rate of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_009</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowRate_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User see rates and comments of house </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System shows rates and comments of house </t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_010</t>
+  </si>
+  <si>
+    <t>Show report button when input is not empty</t>
+  </si>
+  <si>
+    <t>User see the button and can click</t>
+  </si>
+  <si>
+    <t>System shows report button</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_011</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ReportValidation_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ReportValidation_002</t>
+  </si>
+  <si>
+    <t>Disable rate button when input is empty</t>
+  </si>
+  <si>
+    <t>1. Leave the input box empty</t>
+  </si>
+  <si>
+    <t>System disables rate button</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_RateValidation_002</t>
+  </si>
+  <si>
+    <t>Show rate button when input is not empty</t>
+  </si>
+  <si>
+    <t>1. Input into the input box empty</t>
+  </si>
+  <si>
+    <t>System shows rate button</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_012</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_RateValidation_001</t>
+  </si>
+  <si>
+    <t>1. Open report modal
+2. Input into the input box empty</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_013</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowRateAlert_001</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_014</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowRateAlert_002</t>
+  </si>
+  <si>
+    <t>Click rate button when not logged in</t>
+  </si>
+  <si>
+    <t>Click rate button when  logged in</t>
+  </si>
+  <si>
+    <t>1. Do not login the system
+2. Input data
+3. Click on rate button</t>
+  </si>
+  <si>
+    <t>1. Login the system
+2. Input data
+3. Click on rate button</t>
+  </si>
+  <si>
+    <t>User see success alert when click rate button</t>
+  </si>
+  <si>
+    <t>User see warning alert when click rate button</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowTotallyAvailableRoom_001</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_015</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_016</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_017</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_018</t>
+  </si>
+  <si>
+    <t>Verify the show totally available room of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t>Verify the show partially available room of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t>Verify the show available slot of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t>User see partially available room</t>
+  </si>
+  <si>
+    <t>User see totally available room</t>
+  </si>
+  <si>
+    <t>System shows the partially available room</t>
+  </si>
+  <si>
+    <t>System shows partially available room</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowAvailableSlot_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System shows available slot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User seeavailable slot </t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowListAvailableRoom_001</t>
+  </si>
+  <si>
+    <t>Verify the show list available room of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User see list available room </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System shows the list available room </t>
+  </si>
+  <si>
+    <t xml:space="preserve">System shows list available room </t>
+  </si>
+  <si>
+    <t>System shows totally available room</t>
+  </si>
+  <si>
+    <t>System shows the totally available room</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowPartiallyAvailableRoom_001</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_019</t>
+  </si>
+  <si>
+    <t>Verify the show tooltip of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowTooltip_001</t>
+  </si>
+  <si>
+    <t>Hover icon in list room</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_020</t>
+  </si>
+  <si>
+    <t>Verify the navigate to room detail of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t>User navigate to room detail</t>
+  </si>
+  <si>
+    <t>System navigates to room detail</t>
+  </si>
+  <si>
+    <t>Click row of table</t>
+  </si>
+  <si>
+    <t>1. Click row of table</t>
+  </si>
+  <si>
+    <t>1. Hover icon in list room</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_Navigate_001</t>
+  </si>
+  <si>
+    <t>Verify the back to previous of house functionality of House Detail</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_Back_001</t>
+  </si>
+  <si>
+    <t>Click link on top of page</t>
+  </si>
+  <si>
+    <t>1. Click link on top of page</t>
+  </si>
+  <si>
+    <t>User back to previous page</t>
+  </si>
+  <si>
+    <t>System backs to previous page</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_021</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -501,7 +882,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -556,6 +937,15 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -891,29 +1281,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31288BE-C39C-4126-8684-B1EA1FAE63A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="32.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.90625" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="4" max="4" width="15.36328125" customWidth="1"/>
+    <col min="5" max="5" width="32.36328125" customWidth="1"/>
+    <col min="6" max="6" width="16.90625" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="91.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D2" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
@@ -928,7 +1318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>41</v>
       </c>
@@ -943,12 +1333,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="11" t="s">
         <v>45</v>
       </c>
@@ -962,7 +1352,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="19" t="s">
         <v>44</v>
       </c>
@@ -976,7 +1366,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="19">
         <v>44603</v>
       </c>
@@ -990,51 +1380,51 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="19"/>
       <c r="E12" s="14"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="19"/>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="19"/>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="19"/>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="19"/>
       <c r="E16" s="14"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="19"/>
       <c r="E17" s="14"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="19"/>
       <c r="E18" s="14"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="19"/>
       <c r="E19" s="14"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="19"/>
       <c r="E20" s="14"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="19"/>
       <c r="E21" s="14"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="19"/>
       <c r="E22" s="14"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="20"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -1048,32 +1438,32 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA5AA972-DFB1-40B4-AEFA-DB3883430545}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1081,7 +1471,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1101,7 +1491,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1125,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1133,7 +1523,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1141,7 +1531,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1185,7 +1575,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1201,7 +1591,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1217,7 +1607,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1233,7 +1623,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1249,7 +1639,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1265,7 +1655,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1281,7 +1671,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1297,7 +1687,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1313,7 +1703,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1329,7 +1719,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1345,7 +1735,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1361,7 +1751,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1377,7 +1767,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1393,7 +1783,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1415,32 +1805,32 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724366A5-878B-4ED6-A78B-66A2030F69F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1448,7 +1838,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1468,7 +1858,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1492,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1500,7 +1890,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1508,7 +1898,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1552,7 +1942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1568,7 +1958,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1584,7 +1974,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1600,7 +1990,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1616,7 +2006,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1632,7 +2022,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1648,7 +2038,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1664,7 +2054,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1680,7 +2070,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1696,7 +2086,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1712,7 +2102,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1728,7 +2118,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1744,7 +2134,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1760,7 +2150,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1782,46 +2172,46 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D15423-BFD1-49B1-9AC6-A93AC985919D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A783D3-2F75-4808-BD69-9252C407DFB4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1829,7 +2219,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1849,7 +2239,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1873,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1881,7 +2271,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1889,7 +2279,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1933,7 +2323,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1949,7 +2339,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1965,7 +2355,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1981,7 +2371,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1997,7 +2387,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2013,7 +2403,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2029,7 +2419,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2045,7 +2435,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2061,7 +2451,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2077,7 +2467,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2093,7 +2483,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2109,7 +2499,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2125,7 +2515,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2141,7 +2531,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2163,46 +2553,46 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40266175-311B-4BE6-A383-6E85CEC9752E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2210,7 +2600,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2230,7 +2620,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2254,7 +2644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2262,7 +2652,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2270,7 +2660,7 @@
         <v>44692</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -2314,7 +2704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>56</v>
       </c>
@@ -2358,7 +2748,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
         <v>56</v>
       </c>
@@ -2402,7 +2792,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
         <v>56</v>
       </c>
@@ -2446,7 +2836,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
         <v>56</v>
       </c>
@@ -2490,7 +2880,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2506,7 +2896,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2522,7 +2912,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2538,7 +2928,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2554,7 +2944,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2570,7 +2960,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2586,7 +2976,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2602,7 +2992,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2618,7 +3008,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -2634,7 +3024,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -2657,40 +3047,982 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{390F2A9F-4E2C-4E2F-ABD3-049540B295E0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44753</v>
+      </c>
+      <c r="E3" s="17">
+        <f>COUNTIF(K8:K28,"Pass")</f>
+        <v>21</v>
+      </c>
+      <c r="F3" s="17">
+        <f>COUNTIF(K8:K28,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="17">
+        <f>COUNTIF(K8:K28,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="17">
+        <f>COUNTA(K8:K28)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44845</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="27" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A8" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="26"/>
+      <c r="N8" s="23"/>
+    </row>
+    <row r="9" spans="1:14" s="27" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="K9" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" s="26"/>
+      <c r="N9" s="23"/>
+    </row>
+    <row r="10" spans="1:14" s="27" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="K10" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="26"/>
+      <c r="N10" s="23"/>
+    </row>
+    <row r="11" spans="1:14" s="27" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="26"/>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="12" spans="1:14" s="27" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="K12" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" s="26"/>
+      <c r="N12" s="23"/>
+    </row>
+    <row r="13" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+    </row>
+    <row r="14" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="K14" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+    </row>
+    <row r="15" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="K15" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+    </row>
+    <row r="16" spans="1:14" s="28" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="K16" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+    </row>
+    <row r="17" spans="1:14" s="28" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+    </row>
+    <row r="18" spans="1:14" s="27" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="K18" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M18" s="26"/>
+      <c r="N18" s="23"/>
+    </row>
+    <row r="19" spans="1:14" s="27" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" s="26"/>
+      <c r="N19" s="23"/>
+    </row>
+    <row r="20" spans="1:14" s="27" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" s="26"/>
+      <c r="N20" s="23"/>
+    </row>
+    <row r="21" spans="1:14" s="27" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21" s="26"/>
+      <c r="N21" s="23"/>
+    </row>
+    <row r="22" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="K22" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+    </row>
+    <row r="23" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="J23" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="K23" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+    </row>
+    <row r="24" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="J24" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="K24" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L24" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+    </row>
+    <row r="25" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="I25" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="J25" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+    </row>
+    <row r="26" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>180</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F26" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="I26" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="J26" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="K26" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+    </row>
+    <row r="27" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="K27" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+    </row>
+    <row r="28" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="I28" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="J28" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L28" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2710,12 +4042,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>44753</v>
+        <v>44815</v>
       </c>
       <c r="E3" s="17">
         <f>COUNTIF(K8:K11,"Pass")</f>
@@ -2734,7 +4066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2742,7 +4074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -2750,7 +4082,7 @@
         <v>44845</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -2794,7 +4126,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2810,7 +4142,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2826,7 +4158,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2842,7 +4174,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2858,7 +4190,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2874,7 +4206,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2890,7 +4222,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2906,7 +4238,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2922,7 +4254,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -2938,7 +4270,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2954,7 +4286,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2970,7 +4302,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2986,7 +4318,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -3002,7 +4334,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -3023,46 +4355,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9DAF7B-F216-485C-A737-CE6543350613}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>39</v>
@@ -3077,12 +4409,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>44815</v>
+        <v>44845</v>
       </c>
       <c r="E3" s="17">
         <f>COUNTIF(K8:K11,"Pass")</f>
@@ -3101,7 +4433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3109,15 +4441,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>44845</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>44906</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -3161,7 +4493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -3177,7 +4509,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -3193,7 +4525,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -3209,7 +4541,7 @@
       <c r="M10" s="5"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -3225,7 +4557,7 @@
       <c r="M11" s="5"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -3241,7 +4573,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -3257,7 +4589,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -3273,7 +4605,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -3289,7 +4621,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -3305,7 +4637,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -3321,7 +4653,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -3337,7 +4669,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -3353,7 +4685,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -3369,7 +4701,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -3390,418 +4722,51 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFAD3FF7-16E1-4231-B6B4-F5A8EE2491F1}">
-  <dimension ref="A1:N21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5546875" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" customWidth="1"/>
-    <col min="11" max="11" width="8.109375" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>44845</v>
-      </c>
-      <c r="E3" s="17">
-        <f>COUNTIF(K8:K11,"Pass")</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="17">
-        <f>COUNTIF(K8:K11,"Fail")</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="17">
-        <f>COUNTIF(K8:K11,"Untested")</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="17">
-        <f>COUNTA(K8:K11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>44906</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE6BAC9-101B-4E92-9129-5215F08B3B25}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6700F7F-1AC6-48E9-B606-49A22884B31C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8BA7C9D-4811-4DBD-A294-1765E19BD7AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2560414D-76E7-40C1-9529-E439F49BDB5A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
(Integration Test) Room Detail
</commit_message>
<xml_diff>
--- a/Documentation/FHF_TestCases.xlsx
+++ b/Documentation/FHF_TestCases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="213">
   <si>
     <t>Project Name</t>
   </si>
@@ -665,9 +665,6 @@
     <t>TC_FHF_HouseDetail_Navigate_001</t>
   </si>
   <si>
-    <t>Verify the back to previous of house functionality of House Detail</t>
-  </si>
-  <si>
     <t>TC_FHF_HouseDetail_Back_001</t>
   </si>
   <si>
@@ -684,6 +681,54 @@
   </si>
   <si>
     <t>TS_FHF_HouseDetail_021</t>
+  </si>
+  <si>
+    <t>User see images of room</t>
+  </si>
+  <si>
+    <t>System shows the images of room</t>
+  </si>
+  <si>
+    <t>Verify the show image of room functionality of Room Detail</t>
+  </si>
+  <si>
+    <t>TC_FHF_RoomDetail_ShowRoomImage_001</t>
+  </si>
+  <si>
+    <t>Verify the show information of room functionality of Room Detail</t>
+  </si>
+  <si>
+    <t>TC_FHF_RoomDetail_ShowRoomInformation_001</t>
+  </si>
+  <si>
+    <t>User see information of room</t>
+  </si>
+  <si>
+    <t>System shows the information of room</t>
+  </si>
+  <si>
+    <t>TS_FHF_RoomDetail_001</t>
+  </si>
+  <si>
+    <t>TS_FHF_RoomDetail_002</t>
+  </si>
+  <si>
+    <t>TS_FHF_RoomDetail_003</t>
+  </si>
+  <si>
+    <t>Verify the detail landlord of house functionality of Room Detail</t>
+  </si>
+  <si>
+    <t>TC_FHF_RoomDetail_ShowLandlord_001</t>
+  </si>
+  <si>
+    <t>Verify the back to previous of page functionality of Room Detail</t>
+  </si>
+  <si>
+    <t>TC_FHF_RoomDetail_Back_001</t>
+  </si>
+  <si>
+    <t>Verify the back to previous of page functionality of House Detail</t>
   </si>
 </sst>
 </file>
@@ -3050,8 +3095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3946,32 +3991,32 @@
     </row>
     <row r="28" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B28" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="C28" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="D28" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="E28" s="24" t="s">
         <v>193</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>194</v>
       </c>
       <c r="F28" s="24" t="s">
         <v>31</v>
       </c>
       <c r="G28" s="24"/>
       <c r="H28" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I28" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="I28" s="24" t="s">
-        <v>196</v>
-      </c>
       <c r="J28" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K28" s="29" t="s">
         <v>39</v>
@@ -3992,8 +4037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4051,7 +4096,7 @@
       </c>
       <c r="E3" s="17">
         <f>COUNTIF(K8:K11,"Pass")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F3" s="17">
         <f>COUNTIF(K8:K11,"Fail")</f>
@@ -4063,7 +4108,7 @@
       </c>
       <c r="H3" s="17">
         <f>COUNTA(K8:K11)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -4126,69 +4171,157 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="3"/>
+    <row r="8" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+    </row>
+    <row r="9" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+    </row>
+    <row r="10" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+    </row>
+    <row r="11" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>

</xml_diff>

<commit_message>
(Integration Test) Manage Landlords
</commit_message>
<xml_diff>
--- a/Documentation/FHF_TestCases.xlsx
+++ b/Documentation/FHF_TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" tabRatio="891" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" tabRatio="891" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="301">
   <si>
     <t>Project Name</t>
   </si>
@@ -729,6 +729,271 @@
   </si>
   <si>
     <t>Verify the back to previous of page functionality of House Detail</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_001</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_002</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_003</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_004</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_005</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_006</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_007</t>
+  </si>
+  <si>
+    <t>Verify the show total house functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_ShowTotalHouse_001</t>
+  </si>
+  <si>
+    <t>Verify the show available house functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>System shows number of total house</t>
+  </si>
+  <si>
+    <t>System shows number of available house</t>
+  </si>
+  <si>
+    <t>User see number of total house</t>
+  </si>
+  <si>
+    <t>User see number of available house</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_ShowAvailableHouse_001</t>
+  </si>
+  <si>
+    <t>Verify the show total room functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>User see number of total room</t>
+  </si>
+  <si>
+    <t>System shows number of total room</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_ShowTotalRoom_001</t>
+  </si>
+  <si>
+    <t>Verify the show available room functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>User see number of available room</t>
+  </si>
+  <si>
+    <t>System shows number of available room</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_ShowAvailableRoom_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_ShowTotalCapacity_001</t>
+  </si>
+  <si>
+    <t>Verify the show total capacity functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>User see number of total capacity</t>
+  </si>
+  <si>
+    <t>System shows number of total capacity</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_ShowAvailableCapacity_001</t>
+  </si>
+  <si>
+    <t>Verify the show available capacity functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>User see number of available capacity</t>
+  </si>
+  <si>
+    <t>System shows number of available capacity</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_ShowListLandlords_001</t>
+  </si>
+  <si>
+    <t>Verify the list landlords functionality of List Landlords</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User see list landlords </t>
+  </si>
+  <si>
+    <t>System shows the list landlords</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_008</t>
+  </si>
+  <si>
+    <t>Verify the show total house of each landlord functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>User see number of total house of each landlord</t>
+  </si>
+  <si>
+    <t>System shows number of total house of each landlord</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_ShowTotalHouse_002</t>
+  </si>
+  <si>
+    <t>Verify the show total room of each landlord functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>User see number of total room of each landlord</t>
+  </si>
+  <si>
+    <t>System shows number of total room of each landlord</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_ShowTotalRoom_002</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_009</t>
+  </si>
+  <si>
+    <t>User see number of available room of each landlord</t>
+  </si>
+  <si>
+    <t>System shows number of available room of each landlord</t>
+  </si>
+  <si>
+    <t>Verify the show available room of each landlord functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_ShowAvailableRoom_002</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_010</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_011</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_012</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_013</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_014</t>
+  </si>
+  <si>
+    <t>Verify the Search by Name functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_SearchName_004</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_SearchName_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_SearchName_002</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_SearchName_003</t>
+  </si>
+  <si>
+    <t>System displays a message indicating that there are no Landlords containing the searched value</t>
+  </si>
+  <si>
+    <t>System displays 
+the list of Landlords containing the searched value</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_015</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_016</t>
+  </si>
+  <si>
+    <t>Verify the show tooltip of house functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>Verify the navigate to room detail of house functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_ShowTooltip_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_Navigate_001</t>
+  </si>
+  <si>
+    <t>Hover icon in list landlords</t>
+  </si>
+  <si>
+    <t>User see description of this icon</t>
+  </si>
+  <si>
+    <t>System shows the description of this icon</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_022</t>
+  </si>
+  <si>
+    <t>Verify the show phone number functionality of House Detail</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_ShowPhoneNumber_001</t>
+  </si>
+  <si>
+    <t>Click show phone number button</t>
+  </si>
+  <si>
+    <t>1. Click show phone number button</t>
+  </si>
+  <si>
+    <t>User see the phone number of the landlord</t>
+  </si>
+  <si>
+    <t>System shows the phone number of the landlord</t>
+  </si>
+  <si>
+    <t>TS_FHF_HouseDetail_023</t>
+  </si>
+  <si>
+    <t>Verify the navigate to landlord facebook functionality of House Detail</t>
+  </si>
+  <si>
+    <t>TC_FHF_HouseDetail_Navigate_002</t>
+  </si>
+  <si>
+    <t>Click link facebook of landlord</t>
+  </si>
+  <si>
+    <t>1. Click link facebook of landlord</t>
+  </si>
+  <si>
+    <t>User navigate to landlord facebook</t>
+  </si>
+  <si>
+    <t>System navigates to landlord facebook</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListLandlords_017</t>
+  </si>
+  <si>
+    <t>Verify the navigate to landlord facebook functionality of List Landlords</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListLandlords_Navigate_002</t>
+  </si>
+  <si>
+    <t>TS_FHF_RoomDetail_004</t>
   </si>
 </sst>
 </file>
@@ -927,7 +1192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -987,9 +1252,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2615,8 +2886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3093,10 +3364,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3419,7 +3690,7 @@
       <c r="M12" s="26"/>
       <c r="N12" s="23"/>
     </row>
-    <row r="13" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="24" t="s">
         <v>108</v>
       </c>
@@ -3448,7 +3719,7 @@
       <c r="J13" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L13" s="24" t="s">
@@ -3457,7 +3728,7 @@
       <c r="M13" s="24"/>
       <c r="N13" s="24"/>
     </row>
-    <row r="14" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="24" t="s">
         <v>114</v>
       </c>
@@ -3486,7 +3757,7 @@
       <c r="J14" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="K14" s="29" t="s">
+      <c r="K14" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L14" s="24" t="s">
@@ -3495,7 +3766,7 @@
       <c r="M14" s="24"/>
       <c r="N14" s="24"/>
     </row>
-    <row r="15" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
         <v>118</v>
       </c>
@@ -3524,7 +3795,7 @@
       <c r="J15" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="K15" s="29" t="s">
+      <c r="K15" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L15" s="24" t="s">
@@ -3533,7 +3804,7 @@
       <c r="M15" s="24"/>
       <c r="N15" s="24"/>
     </row>
-    <row r="16" spans="1:14" s="28" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" s="29" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
         <v>125</v>
       </c>
@@ -3562,7 +3833,7 @@
       <c r="J16" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="K16" s="29" t="s">
+      <c r="K16" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L16" s="24" t="s">
@@ -3571,7 +3842,7 @@
       <c r="M16" s="24"/>
       <c r="N16" s="24"/>
     </row>
-    <row r="17" spans="1:14" s="28" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" s="29" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
         <v>129</v>
       </c>
@@ -3600,7 +3871,7 @@
       <c r="J17" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L17" s="24" t="s">
@@ -3761,7 +4032,7 @@
       <c r="M21" s="26"/>
       <c r="N21" s="23"/>
     </row>
-    <row r="22" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="24" t="s">
         <v>157</v>
       </c>
@@ -3790,7 +4061,7 @@
       <c r="J22" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="K22" s="29" t="s">
+      <c r="K22" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L22" s="24" t="s">
@@ -3799,7 +4070,7 @@
       <c r="M22" s="24"/>
       <c r="N22" s="24"/>
     </row>
-    <row r="23" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="24" t="s">
         <v>158</v>
       </c>
@@ -3828,7 +4099,7 @@
       <c r="J23" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="K23" s="29" t="s">
+      <c r="K23" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L23" s="24" t="s">
@@ -3837,7 +4108,7 @@
       <c r="M23" s="24"/>
       <c r="N23" s="24"/>
     </row>
-    <row r="24" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="24" t="s">
         <v>159</v>
       </c>
@@ -3866,7 +4137,7 @@
       <c r="J24" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="K24" s="29" t="s">
+      <c r="K24" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L24" s="24" t="s">
@@ -3875,7 +4146,7 @@
       <c r="M24" s="24"/>
       <c r="N24" s="24"/>
     </row>
-    <row r="25" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="24" t="s">
         <v>160</v>
       </c>
@@ -3904,7 +4175,7 @@
       <c r="J25" s="24" t="s">
         <v>175</v>
       </c>
-      <c r="K25" s="29" t="s">
+      <c r="K25" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L25" s="24" t="s">
@@ -3913,7 +4184,7 @@
       <c r="M25" s="24"/>
       <c r="N25" s="24"/>
     </row>
-    <row r="26" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="24" t="s">
         <v>179</v>
       </c>
@@ -3934,15 +4205,15 @@
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="24" t="s">
-        <v>173</v>
+        <v>281</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>174</v>
+        <v>282</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="K26" s="29" t="s">
+        <v>282</v>
+      </c>
+      <c r="K26" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L26" s="24" t="s">
@@ -3951,7 +4222,7 @@
       <c r="M26" s="24"/>
       <c r="N26" s="24"/>
     </row>
-    <row r="27" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="24" t="s">
         <v>183</v>
       </c>
@@ -3980,7 +4251,7 @@
       <c r="J27" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="K27" s="29" t="s">
+      <c r="K27" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L27" s="24" t="s">
@@ -3989,7 +4260,7 @@
       <c r="M27" s="24"/>
       <c r="N27" s="24"/>
     </row>
-    <row r="28" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="24" t="s">
         <v>196</v>
       </c>
@@ -4018,7 +4289,7 @@
       <c r="J28" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="K28" s="29" t="s">
+      <c r="K28" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L28" s="24" t="s">
@@ -4026,6 +4297,82 @@
       </c>
       <c r="M28" s="24"/>
       <c r="N28" s="24"/>
+    </row>
+    <row r="29" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="J29" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="K29" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+    </row>
+    <row r="30" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="J30" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="K30" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L30" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4037,8 +4384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4171,7 +4518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="24" t="s">
         <v>205</v>
       </c>
@@ -4200,7 +4547,7 @@
       <c r="J8" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L8" s="24" t="s">
@@ -4209,7 +4556,7 @@
       <c r="M8" s="24"/>
       <c r="N8" s="24"/>
     </row>
-    <row r="9" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="24" t="s">
         <v>206</v>
       </c>
@@ -4238,7 +4585,7 @@
       <c r="J9" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L9" s="24" t="s">
@@ -4247,7 +4594,7 @@
       <c r="M9" s="24"/>
       <c r="N9" s="24"/>
     </row>
-    <row r="10" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="24" t="s">
         <v>207</v>
       </c>
@@ -4276,7 +4623,7 @@
       <c r="J10" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L10" s="24" t="s">
@@ -4285,9 +4632,9 @@
       <c r="M10" s="24"/>
       <c r="N10" s="24"/>
     </row>
-    <row r="11" spans="1:14" s="28" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
-        <v>101</v>
+        <v>300</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>210</v>
@@ -4314,7 +4661,7 @@
       <c r="J11" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="K11" s="29" t="s">
+      <c r="K11" s="30" t="s">
         <v>39</v>
       </c>
       <c r="L11" s="24" t="s">
@@ -4883,12 +5230,813 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44845</v>
+      </c>
+      <c r="E3" s="17">
+        <f>COUNTIF(K8:K11,"Pass")</f>
+        <v>4</v>
+      </c>
+      <c r="F3" s="17">
+        <f>COUNTIF(K8:K11,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="17">
+        <f>COUNTIF(K8:K11,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="17">
+        <f>COUNTA(K8:K11)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44906</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+    </row>
+    <row r="9" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="K9" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+    </row>
+    <row r="10" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="K10" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+    </row>
+    <row r="11" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="K11" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+    </row>
+    <row r="12" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="K12" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+    </row>
+    <row r="13" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="K13" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+    </row>
+    <row r="14" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="K14" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+    </row>
+    <row r="15" spans="1:14" s="29" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="K15" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+    </row>
+    <row r="16" spans="1:14" s="29" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A16" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="K16" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+    </row>
+    <row r="17" spans="1:14" s="29" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="K17" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+    </row>
+    <row r="18" spans="1:14" s="28" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="K18" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M18" s="31">
+        <v>44631</v>
+      </c>
+      <c r="N18" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="28" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="K19" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" s="31">
+        <v>44631</v>
+      </c>
+      <c r="N19" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="28" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="K20" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" s="31">
+        <v>44631</v>
+      </c>
+      <c r="N20" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="28" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="J21" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="K21" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21" s="31">
+        <v>44631</v>
+      </c>
+      <c r="N21" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="K22" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+    </row>
+    <row r="23" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>279</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="J23" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="K23" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+    </row>
+    <row r="24" spans="1:14" s="29" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A24" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="J24" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="K24" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L24" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M24" s="24"/>
+      <c r="N24" s="24"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
(Integration Test) List Houses
</commit_message>
<xml_diff>
--- a/Documentation/FHF_TestCases.xlsx
+++ b/Documentation/FHF_TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" tabRatio="891" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580" tabRatio="891" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="358">
   <si>
     <t>Project Name</t>
   </si>
@@ -994,6 +994,177 @@
   </si>
   <si>
     <t>TS_FHF_RoomDetail_004</t>
+  </si>
+  <si>
+    <t>System navigates to list houses of this landlord</t>
+  </si>
+  <si>
+    <t>Verify the show total house functionality of List Houses</t>
+  </si>
+  <si>
+    <t>Verify the show available house functionality of List Houses</t>
+  </si>
+  <si>
+    <t>Verify the show total room functionality of List Houses</t>
+  </si>
+  <si>
+    <t>Verify the show available room functionality of List Houses</t>
+  </si>
+  <si>
+    <t>Verify the show total capacity functionality of List Houses</t>
+  </si>
+  <si>
+    <t>Verify the show available capacity functionality of List Houses</t>
+  </si>
+  <si>
+    <t>Verify the list landlords functionality of List Houses</t>
+  </si>
+  <si>
+    <t>Verify the Search by Name functionality of List Houses</t>
+  </si>
+  <si>
+    <t>Verify the show tooltip of house functionality of List Houses</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_016</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_015</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_014</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_013</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_012</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_011</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_010</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_009</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_008</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_007</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_006</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_005</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_004</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_003</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_002</t>
+  </si>
+  <si>
+    <t>TS_FHF_ListHouses_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_ShowTotalHouse_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_ShowAvailableHouse_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_ShowTotalRoom_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_ShowAvailableRoom_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_ShowTotalCapacity_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_ShowAvailableCapacity_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_ShowListHouses_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_SearchName_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_SearchName_002</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_SearchName_003</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_SearchName_004</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_ShowTooltip_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_Navigate_001</t>
+  </si>
+  <si>
+    <t>Verify the show totally available room of each house functionality of List Houses</t>
+  </si>
+  <si>
+    <t>User see number of totally available room of each house</t>
+  </si>
+  <si>
+    <t>System shows number of totally available room of each house</t>
+  </si>
+  <si>
+    <t>Verify the show partially available room of each house functionality of List Houses</t>
+  </si>
+  <si>
+    <t>User see number of partially available room of each house</t>
+  </si>
+  <si>
+    <t>System shows number of partially available room of each house</t>
+  </si>
+  <si>
+    <t>Verify the show available capacity of each house functionality of List Houses</t>
+  </si>
+  <si>
+    <t>User see number of available capacity of each house</t>
+  </si>
+  <si>
+    <t>System shows number of available capacity of each house</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_ShowTotallyAvailableRoom_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_ListHouses_ShowPartiallyAvailableRoom_001</t>
+  </si>
+  <si>
+    <t>Hover icon in list houses</t>
+  </si>
+  <si>
+    <t>1. Hover icon in list houses</t>
+  </si>
+  <si>
+    <t>1. Hover icon in list landlords</t>
+  </si>
+  <si>
+    <t>Verify the navigate to house detail of house functionality of List Houses</t>
+  </si>
+  <si>
+    <t>User navigate to house detail</t>
+  </si>
+  <si>
+    <t>System navigates to house detail</t>
+  </si>
+  <si>
+    <t>User navigate to list houses of this landlord</t>
   </si>
 </sst>
 </file>
@@ -5232,8 +5403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5290,20 +5461,20 @@
         <v>44845</v>
       </c>
       <c r="E3" s="17">
-        <f>COUNTIF(K8:K11,"Pass")</f>
-        <v>4</v>
+        <f>COUNTIF(K8:K24,"Pass")</f>
+        <v>17</v>
       </c>
       <c r="F3" s="17">
-        <f>COUNTIF(K8:K11,"Fail")</f>
+        <f>COUNTIF(K8:K24,"Fail")</f>
         <v>0</v>
       </c>
       <c r="G3" s="17">
-        <f>COUNTIF(K8:K11,"Untested")</f>
+        <f>COUNTIF(K8:K24,"Untested")</f>
         <v>0</v>
       </c>
       <c r="H3" s="17">
-        <f>COUNTA(K8:K11)</f>
-        <v>4</v>
+        <f>COUNTA(K8:K24)</f>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -5936,7 +6107,7 @@
         <v>280</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>189</v>
+        <v>353</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>31</v>
@@ -5981,13 +6152,13 @@
       </c>
       <c r="G23" s="24"/>
       <c r="H23" s="24" t="s">
-        <v>185</v>
+        <v>357</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>186</v>
+        <v>301</v>
       </c>
       <c r="J23" s="24" t="s">
-        <v>186</v>
+        <v>301</v>
       </c>
       <c r="K23" s="30" t="s">
         <v>39</v>
@@ -6043,12 +6214,775 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.36328125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="11" max="11" width="8.08984375" customWidth="1"/>
+    <col min="12" max="12" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44876</v>
+      </c>
+      <c r="E3" s="17">
+        <f>COUNTIF(K8:K23,"Pass")</f>
+        <v>16</v>
+      </c>
+      <c r="F3" s="17">
+        <f>COUNTIF(K8:K23,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="17">
+        <f>COUNTIF(K8:K23,"Untested")</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="17">
+        <f>COUNTA(K8:K23)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44906</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="29" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="24" t="s">
+        <v>326</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>302</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
+    </row>
+    <row r="9" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="24" t="s">
+        <v>325</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="K9" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+    </row>
+    <row r="10" spans="1:14" s="29" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>329</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="K10" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+    </row>
+    <row r="11" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="K11" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+    </row>
+    <row r="12" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="K12" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+    </row>
+    <row r="13" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>332</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="K13" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+    </row>
+    <row r="14" spans="1:14" s="29" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>308</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>333</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="K14" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+    </row>
+    <row r="15" spans="1:14" s="29" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="I15" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="K15" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+    </row>
+    <row r="16" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24" t="s">
+        <v>347</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="K16" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+    </row>
+    <row r="17" spans="1:14" s="29" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>343</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>350</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="J17" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="K17" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+    </row>
+    <row r="18" spans="1:14" s="28" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M18" s="31">
+        <v>44631</v>
+      </c>
+      <c r="N18" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="28" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="K19" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" s="31">
+        <v>44631</v>
+      </c>
+      <c r="N19" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="28" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A20" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" s="31">
+        <v>44631</v>
+      </c>
+      <c r="N20" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="28" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="K21" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21" s="31">
+        <v>44631</v>
+      </c>
+      <c r="N21" s="24" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>310</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>351</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="I22" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="J22" s="24" t="s">
+        <v>282</v>
+      </c>
+      <c r="K22" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+    </row>
+    <row r="23" spans="1:14" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>356</v>
+      </c>
+      <c r="J23" s="24" t="s">
+        <v>356</v>
+      </c>
+      <c r="K23" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Integration Test] Staff Dashboard
</commit_message>
<xml_diff>
--- a/Documentation/FHF_TestCases.xlsx
+++ b/Documentation/FHF_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Semester9\SEP490\fu-house-finder\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF0F0B2-B586-42F0-B65E-9687DC2E19EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72160088-8E01-47E0-9538-BCCE13A7CEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="891" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="891" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1253" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="389">
   <si>
     <t>Project Name</t>
   </si>
@@ -1206,6 +1206,53 @@
   </si>
   <si>
     <t>(Staff) Manage Landlords, List Houses</t>
+  </si>
+  <si>
+    <t>TS_FHF_StaffDashboard_001</t>
+  </si>
+  <si>
+    <t>User Logged in as Staff</t>
+  </si>
+  <si>
+    <t>System displays sum of houses, landlords, capacity &amp; regions</t>
+  </si>
+  <si>
+    <t>TS_FHF_StaffDashboard_002</t>
+  </si>
+  <si>
+    <t>Verify the Numerical Statistics Report functionality of Staff Dashboard</t>
+  </si>
+  <si>
+    <t>Enter the Page to see Numerical Statistics Report</t>
+  </si>
+  <si>
+    <t>1. Enter the Staff Dashboard Page
+2. Scroll down to see the Numerical Statistics Reports</t>
+  </si>
+  <si>
+    <t>User see all Numerical Statistics Reports</t>
+  </si>
+  <si>
+    <t>Verify the Graphical Statistics Report functionality of Staff Dashboard</t>
+  </si>
+  <si>
+    <t>TC_FHF_StaffDashboard_NumericReport_001</t>
+  </si>
+  <si>
+    <t>TC_FHF_StaffDashboard_GraphicReport_001</t>
+  </si>
+  <si>
+    <t>Enter the Page to see Graphical Statistics Report</t>
+  </si>
+  <si>
+    <t>1. Enter the Staff Dashboard Page
+2. Scroll down to see the Graphical Statistics Reports</t>
+  </si>
+  <si>
+    <t>User see all Graphical Statistics Reports</t>
+  </si>
+  <si>
+    <t>System displays graphical statistics of houses, rooms, capacity, landlords, orders &amp; reports</t>
   </si>
 </sst>
 </file>
@@ -1404,7 +1451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1475,6 +1522,21 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1812,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3869,7 +3931,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4349,12 +4411,12 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
@@ -5459,7 +5521,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6679,13 +6741,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
@@ -6738,7 +6800,7 @@
       </c>
       <c r="E3" s="16">
         <f>COUNTIF(K8:K11,"Pass")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F3" s="16">
         <f>COUNTIF(K8:K11,"Fail")</f>
@@ -6750,7 +6812,7 @@
       </c>
       <c r="H3" s="16">
         <f>COUNTA(K8:K11)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -6813,229 +6875,281 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="2"/>
+    <row r="8" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>378</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>379</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="29">
+        <v>44907</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>375</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23" t="s">
+        <v>387</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>388</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>388</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="29">
+        <v>44907</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="2"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="35"/>
+      <c r="N10" s="32"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="2"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="35"/>
+      <c r="N11" s="32"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7046,7 +7160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[Integration Test] Home Page
Filter by Distance: finish
</commit_message>
<xml_diff>
--- a/Documentation/FHF_TestCases.xlsx
+++ b/Documentation/FHF_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Semester9\SEP490\fu-house-finder\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A46810B-239C-4BEA-9189-5489B692C3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8817A882-B214-4366-A718-1A1551814ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="891" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="490">
   <si>
     <t>Project Name</t>
   </si>
@@ -1849,6 +1849,362 @@
   </si>
   <si>
     <t>System doesn’t change</t>
+  </si>
+  <si>
+    <t>TC_FHF_Home_FilterByDistance_003</t>
+  </si>
+  <si>
+    <t>1. Select a Campus from the Dropdown
+2. Input invalid Distance - From
+3. Input valid Distance - To
+4. Click "Áp dụng"</t>
+  </si>
+  <si>
+    <t>User failed to input text to Form</t>
+  </si>
+  <si>
+    <t>TC_FHF_Home_FilterByDistance_004</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Campus: FU - Hòa Lạc
+Distance - From: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>abc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Distance - To: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Campus: FU - Hòa Lạc
+Distance - From: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Distance - To: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_FHF_Home_FilterByDistance_005</t>
+  </si>
+  <si>
+    <t>Choose a Campus, then input blank Distance</t>
+  </si>
+  <si>
+    <t>Choose a Campus, then input invalid Distance</t>
+  </si>
+  <si>
+    <t>1. Select a Campus from the Dropdown
+2. Input valid Distance - From
+3. Input invalid Distance - To
+4. Click "Áp dụng"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Campus: FU - Hòa Lạc
+Distance - From: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Distance - To: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <t>System displays alert: "Giá trị nhập vào không hợp lệ!"</t>
+  </si>
+  <si>
+    <t>TC_FHF_Home_FilterByDistance_006</t>
+  </si>
+  <si>
+    <t>1. Select a Campus from the Dropdown
+2. Input invalid Distance - From
+3. Input invalid Distance - To
+4. Click "Áp dụng"</t>
+  </si>
+  <si>
+    <r>
+      <t>Campus: FU - Hòa Lạc
+Distance - From: -</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Distance - To: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+  </si>
+  <si>
+    <t>TC_FHF_Home_FilterByDistance_007</t>
+  </si>
+  <si>
+    <t>Choose a Campus, then input valid Distance but From is larger than To</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Campus: FU - Hòa Lạc
+Distance - From: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Distance - To: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Input Distance but not choosing Campus</t>
+  </si>
+  <si>
+    <t>1. Input valid Distance - From
+2. Input valid Distance - To
+3. Click "Áp dụng"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Distance - From: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Distance - To: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>System displays alert: "Vui lòng chọn Cơ sở bạn học trước!"</t>
+  </si>
+  <si>
+    <t>TC_FHF_Home_FilterByDistance_008</t>
+  </si>
+  <si>
+    <t>TS_FHF_Home_005</t>
+  </si>
+  <si>
+    <t>Verify the Filter by Price functionality of Home Page</t>
+  </si>
+  <si>
+    <t>TC_FHF_Home_FilterByPrice_001</t>
+  </si>
+  <si>
+    <t>Input valid Prices</t>
+  </si>
+  <si>
+    <t>1. Input valid Price - From
+2. Input valid Price - To
+3. Click "Áp dụng"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Price - From: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2000000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Price - To: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3000000</t>
+    </r>
+  </si>
+  <si>
+    <t>User see Houses with Room Price from 2000000 to 3000000 per month</t>
+  </si>
+  <si>
+    <t>System displays a list of Houses with Room Price from 2000000 to 3000000 per month</t>
   </si>
 </sst>
 </file>
@@ -4528,10 +4884,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4664,7 +5020,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>55</v>
       </c>
@@ -4752,7 +5108,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>55</v>
       </c>
@@ -4972,7 +5328,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="135" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>419</v>
       </c>
@@ -5104,7 +5460,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
         <v>439</v>
       </c>
@@ -5148,7 +5504,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
         <v>439</v>
       </c>
@@ -5159,7 +5515,7 @@
         <v>453</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>442</v>
+        <v>466</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>457</v>
@@ -5192,21 +5548,441 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+    <row r="20" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>440</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>459</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>460</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>463</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>461</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>458</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>458</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M20" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="N20" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>440</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>462</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>460</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="23" t="s">
+        <v>464</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>455</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="J21" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="K21" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M21" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="N21" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>440</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>465</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>468</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>469</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>455</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="K22" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="N22" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>440</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>471</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>467</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>472</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>473</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>455</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="J23" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L23" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="N23" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>440</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>474</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>475</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>456</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>476</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>455</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>470</v>
+      </c>
+      <c r="K24" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="N24" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>440</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>477</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>478</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="23" t="s">
+        <v>479</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>455</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="J25" s="23" t="s">
+        <v>480</v>
+      </c>
+      <c r="K25" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>482</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>483</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>484</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>485</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>486</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>487</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>488</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="J26" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="K26" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="N26" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="22"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="22"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="22"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="22"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="22"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="22"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="22"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="22"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="22"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="22"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[Document] (Integration Test) Home Page
Order by
</commit_message>
<xml_diff>
--- a/Documentation/FHF_TestCases.xlsx
+++ b/Documentation/FHF_TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Semester9\SEP490\fu-house-finder\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE66401E-C7DF-4223-B1B9-985B6F4CD81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81AC73E-BC4E-4767-BE94-B8535DAC37A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="891" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1890" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1978" uniqueCount="627">
   <si>
     <t>Project Name</t>
   </si>
@@ -2973,6 +2973,153 @@
   </si>
   <si>
     <t>System displays list of Houses with average Rate from 5 Star and up</t>
+  </si>
+  <si>
+    <t>TS_FHF_Home_010</t>
+  </si>
+  <si>
+    <t>Paging</t>
+  </si>
+  <si>
+    <t>Cancel Filter</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Kết hợp Filter, paging &amp; order by, search</t>
+  </si>
+  <si>
+    <t>Verify the Order By functionality of Home Page</t>
+  </si>
+  <si>
+    <t>TC_FHF_Home_OrderBy_001</t>
+  </si>
+  <si>
+    <t>Select an Order value</t>
+  </si>
+  <si>
+    <t>1. Select an Order value from list of Order values</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Order by: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Khoảng cách: Gần đến Xa</t>
+    </r>
+  </si>
+  <si>
+    <t>User sees Houses ordered by the selected Order value</t>
+  </si>
+  <si>
+    <t>System displays list of Houses  ordered by the selected Order value</t>
+  </si>
+  <si>
+    <t>System displays list of Houses ordered by the selected Order value</t>
+  </si>
+  <si>
+    <t>TC_FHF_Home_OrderBy_002</t>
+  </si>
+  <si>
+    <t>TC_FHF_Home_OrderBy_003</t>
+  </si>
+  <si>
+    <t>TC_FHF_Home_OrderBy_004</t>
+  </si>
+  <si>
+    <t>TC_FHF_Home_OrderBy_005</t>
+  </si>
+  <si>
+    <t>TC_FHF_Home_OrderBy_006</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Order by: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Giá: Thấp đến Cao</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Order by: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Giá: Cao đến Thấp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Order by: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Khoảng cách: Xa đến Gần</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Order by: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Đánh giá: Cao đến Thấp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Order by:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Đánh giá: Thấp đến Cao</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3171,7 +3318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -3245,6 +3392,18 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -5652,10 +5811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5712,8 +5871,8 @@
         <v>334</v>
       </c>
       <c r="E3" s="16">
-        <f>COUNTIF(K8:K49,"Pass")</f>
-        <v>42</v>
+        <f>COUNTIF(K8:K54,"Pass")</f>
+        <v>47</v>
       </c>
       <c r="F3" s="16">
         <f>COUNTIF(K8:K11,"Fail")</f>
@@ -7854,6 +8013,338 @@
       </c>
       <c r="N54" s="22" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>609</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>610</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>611</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>612</v>
+      </c>
+      <c r="F55" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G55" s="23" t="s">
+        <v>622</v>
+      </c>
+      <c r="H55" s="23" t="s">
+        <v>614</v>
+      </c>
+      <c r="I55" s="23" t="s">
+        <v>615</v>
+      </c>
+      <c r="J55" s="23" t="s">
+        <v>616</v>
+      </c>
+      <c r="K55" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L55" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M55" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="N55" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="B56" s="23" t="s">
+        <v>609</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>617</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>611</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>612</v>
+      </c>
+      <c r="F56" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" s="23" t="s">
+        <v>623</v>
+      </c>
+      <c r="H56" s="23" t="s">
+        <v>614</v>
+      </c>
+      <c r="I56" s="23" t="s">
+        <v>615</v>
+      </c>
+      <c r="J56" s="23" t="s">
+        <v>616</v>
+      </c>
+      <c r="K56" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L56" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M56" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="N56" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>609</v>
+      </c>
+      <c r="C57" s="23" t="s">
+        <v>618</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>611</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>612</v>
+      </c>
+      <c r="F57" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G57" s="23" t="s">
+        <v>613</v>
+      </c>
+      <c r="H57" s="23" t="s">
+        <v>614</v>
+      </c>
+      <c r="I57" s="23" t="s">
+        <v>615</v>
+      </c>
+      <c r="J57" s="23" t="s">
+        <v>616</v>
+      </c>
+      <c r="K57" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L57" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M57" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="N57" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>609</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>619</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>611</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>612</v>
+      </c>
+      <c r="F58" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G58" s="23" t="s">
+        <v>624</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>614</v>
+      </c>
+      <c r="I58" s="23" t="s">
+        <v>615</v>
+      </c>
+      <c r="J58" s="23" t="s">
+        <v>616</v>
+      </c>
+      <c r="K58" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L58" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="N58" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>609</v>
+      </c>
+      <c r="C59" s="23" t="s">
+        <v>620</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>611</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>612</v>
+      </c>
+      <c r="F59" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>625</v>
+      </c>
+      <c r="H59" s="23" t="s">
+        <v>614</v>
+      </c>
+      <c r="I59" s="23" t="s">
+        <v>615</v>
+      </c>
+      <c r="J59" s="23" t="s">
+        <v>616</v>
+      </c>
+      <c r="K59" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L59" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M59" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="N59" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
+        <v>604</v>
+      </c>
+      <c r="B60" s="23" t="s">
+        <v>609</v>
+      </c>
+      <c r="C60" s="23" t="s">
+        <v>621</v>
+      </c>
+      <c r="D60" s="23" t="s">
+        <v>611</v>
+      </c>
+      <c r="E60" s="23" t="s">
+        <v>612</v>
+      </c>
+      <c r="F60" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G60" s="23" t="s">
+        <v>626</v>
+      </c>
+      <c r="H60" s="23" t="s">
+        <v>614</v>
+      </c>
+      <c r="I60" s="23" t="s">
+        <v>615</v>
+      </c>
+      <c r="J60" s="23" t="s">
+        <v>616</v>
+      </c>
+      <c r="K60" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="L60" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="M60" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="N60" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="33"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="34"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="34"/>
+      <c r="J61" s="34"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="36"/>
+      <c r="N61" s="33"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="33"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="34"/>
+      <c r="H62" s="34"/>
+      <c r="I62" s="34"/>
+      <c r="J62" s="34"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="33"/>
+      <c r="M62" s="36"/>
+      <c r="N62" s="33"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="33"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="34"/>
+      <c r="H63" s="34"/>
+      <c r="I63" s="34"/>
+      <c r="J63" s="34"/>
+      <c r="K63" s="35"/>
+      <c r="L63" s="33"/>
+      <c r="M63" s="36"/>
+      <c r="N63" s="33"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>607</v>
       </c>
     </row>
   </sheetData>
@@ -7867,7 +8358,7 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>